<commit_message>
Today we are going to change the TV, much simpler to what we have already
</commit_message>
<xml_diff>
--- a/Master_Reconciliation_GF.xlsx
+++ b/Master_Reconciliation_GF.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmsou\Documents\mokum.ai\Goldfinger\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAB7320-39BF-47F6-9166-7A0E2996EB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -205,12 +199,6 @@
     <t>11 - RM_11_PRIORITY_SpecifiConLLC_7274_75K</t>
   </si>
   <si>
-    <t>15 - CLOSED_RM_15_SIGNAPAY_SpecifiConLLC_3709_50K</t>
-  </si>
-  <si>
-    <t>2 - RM_2_PAYARC_SpecifiConLLC_9181_55K</t>
-  </si>
-  <si>
     <t>3 - RM_3_NETEVIA_SpecifiConLLC_8884_65K</t>
   </si>
   <si>
@@ -256,6 +244,9 @@
     <t>19 - RM_19_SIGNAPAY_UniquePlusLLC_4137_50K</t>
   </si>
   <si>
+    <t>20 - CLOSED_RM_20_SIGNAPAY_UniquePlusLLC_4129_50K</t>
+  </si>
+  <si>
     <t>25 - RM_25_QUANTUM_UniquePlusLLC_3389_25K</t>
   </si>
   <si>
@@ -290,12 +281,6 @@
   </si>
   <si>
     <t>44 - RM_44_NETEVIA_UniquePlusLLC_9154_65K</t>
-  </si>
-  <si>
-    <t>71 - HOLD_WM_71_PAYSAFE_UniquePlusLLC_9410_50K</t>
-  </si>
-  <si>
-    <t>72 - HOLD_WM_72_PAYSAFE_UniquePlusLLC_9428_50K</t>
   </si>
   <si>
     <t>N</t>
@@ -307,11 +292,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,21 +360,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -427,7 +404,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -461,7 +438,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -496,10 +472,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -672,19 +647,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.1796875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,9 +677,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -718,10 +688,10 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E2">
-        <v>-60.99</v>
+        <v>-309.82</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -730,9 +700,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -741,21 +711,21 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E3">
-        <v>202.01</v>
+        <v>202.52</v>
       </c>
       <c r="F3">
-        <v>177.76</v>
+        <v>144.18</v>
       </c>
       <c r="G3">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -764,21 +734,21 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E4">
-        <v>202.01</v>
+        <v>42.9</v>
       </c>
       <c r="F4">
-        <v>79.400000000000006</v>
+        <v>3.2</v>
       </c>
       <c r="G4">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -787,21 +757,21 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E5">
-        <v>648.36</v>
+        <v>134.45</v>
       </c>
       <c r="F5">
-        <v>473.14</v>
+        <v>491.69</v>
       </c>
       <c r="G5">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -810,21 +780,21 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E6">
-        <v>315.62</v>
+        <v>197.78</v>
       </c>
       <c r="F6">
-        <v>430.9</v>
+        <v>55.54</v>
       </c>
       <c r="G6">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -833,21 +803,21 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E7">
-        <v>117.84</v>
+        <v>18.95</v>
       </c>
       <c r="F7">
-        <v>210.11</v>
+        <v>15.91</v>
       </c>
       <c r="G7">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -856,21 +826,21 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E8">
-        <v>479.47</v>
+        <v>103.12</v>
       </c>
       <c r="F8">
-        <v>967.73</v>
+        <v>424.65</v>
       </c>
       <c r="G8">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -879,21 +849,21 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E9">
-        <v>165.68</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>388.13</v>
+        <v>98.12</v>
       </c>
       <c r="G9">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -902,21 +872,21 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E10">
-        <v>370.54</v>
+        <v>351.59</v>
       </c>
       <c r="F10">
-        <v>1050.3900000000001</v>
+        <v>690.15</v>
       </c>
       <c r="G10">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -925,21 +895,21 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E11">
-        <v>71.28</v>
+        <v>255.4</v>
       </c>
       <c r="F11">
-        <v>625.44000000000005</v>
+        <v>229.21</v>
       </c>
       <c r="G11">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -948,21 +918,21 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E12">
-        <v>443.4</v>
+        <v>430.56</v>
       </c>
       <c r="F12">
-        <v>535.78</v>
+        <v>709.04</v>
       </c>
       <c r="G12">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -971,21 +941,21 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E13">
-        <v>249.34</v>
+        <v>245.72</v>
       </c>
       <c r="F13">
-        <v>1113.6600000000001</v>
+        <v>204.08</v>
       </c>
       <c r="G13">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -994,21 +964,21 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E14">
         <v>103.12</v>
       </c>
       <c r="F14">
-        <v>306.77</v>
+        <v>88.17</v>
       </c>
       <c r="G14">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -1017,21 +987,21 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E15">
-        <v>57.62</v>
+        <v>160.74</v>
       </c>
       <c r="F15">
-        <v>204.79</v>
+        <v>130.02</v>
       </c>
       <c r="G15">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -1040,21 +1010,21 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E16">
-        <v>420.31</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>648.06999999999994</v>
+        <v>49.46</v>
       </c>
       <c r="G16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -1063,21 +1033,21 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E17">
-        <v>37.9</v>
+        <v>18.95</v>
       </c>
       <c r="F17">
-        <v>63.71</v>
+        <v>31.86</v>
       </c>
       <c r="G17">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -1086,21 +1056,21 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E18">
-        <v>392.7</v>
+        <v>179.95</v>
       </c>
       <c r="F18">
-        <v>1355.56</v>
+        <v>307.9</v>
       </c>
       <c r="G18">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1109,21 +1079,21 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E19">
-        <v>529.75</v>
+        <v>524.46</v>
       </c>
       <c r="F19">
-        <v>650.85</v>
+        <v>470.99</v>
       </c>
       <c r="G19">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1132,10 +1102,10 @@
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E20">
-        <v>76.569999999999993</v>
+        <v>-21.55</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1144,9 +1114,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1155,21 +1125,21 @@
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E21">
-        <v>56.85</v>
+        <v>37.9</v>
       </c>
       <c r="F21">
-        <v>47.78</v>
+        <v>15.93</v>
       </c>
       <c r="G21">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1178,21 +1148,21 @@
         <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E22">
-        <v>288.01</v>
+        <v>-21.55</v>
       </c>
       <c r="F22">
-        <v>90.75</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -1201,21 +1171,21 @@
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E23">
-        <v>197.78</v>
+        <v>194.57</v>
       </c>
       <c r="F23">
-        <v>174.04</v>
+        <v>42.1</v>
       </c>
       <c r="G23">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7">
       <c r="A24" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -1224,21 +1194,21 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E24">
-        <v>296.67</v>
+        <v>-146.73</v>
       </c>
       <c r="F24">
-        <v>660.32999999999993</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -1247,21 +1217,21 @@
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E25">
-        <v>367.69</v>
+        <v>255.4</v>
       </c>
       <c r="F25">
-        <v>1307.23</v>
+        <v>350.56</v>
       </c>
       <c r="G25">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1270,21 +1240,21 @@
         <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E26">
-        <v>520.74</v>
+        <v>236.45</v>
       </c>
       <c r="F26">
-        <v>1210.18</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7">
       <c r="A27" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -1293,21 +1263,21 @@
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E27">
-        <v>294.07</v>
+        <v>255.91</v>
       </c>
       <c r="F27">
-        <v>466.21</v>
+        <v>229.73</v>
       </c>
       <c r="G27">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1316,21 +1286,21 @@
         <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E28">
-        <v>192.58</v>
+        <v>154.68</v>
       </c>
       <c r="F28">
-        <v>348.33</v>
+        <v>102.83</v>
       </c>
       <c r="G28">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -1339,21 +1309,21 @@
         <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E29">
-        <v>313.79000000000002</v>
+        <v>-168.28</v>
       </c>
       <c r="F29">
-        <v>1170.8499999999999</v>
+        <v>168.54</v>
       </c>
       <c r="G29">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -1362,21 +1332,21 @@
         <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E30">
-        <v>274.35000000000002</v>
+        <v>470.3</v>
       </c>
       <c r="F30">
-        <v>476.87</v>
+        <v>289.07</v>
       </c>
       <c r="G30">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -1385,21 +1355,21 @@
         <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E31">
-        <v>308.66000000000003</v>
+        <v>591.15</v>
       </c>
       <c r="F31">
-        <v>762.3</v>
+        <v>561.67</v>
       </c>
       <c r="G31">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7">
       <c r="A32" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -1408,21 +1378,21 @@
         <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E32">
         <v>18.95</v>
       </c>
       <c r="F32">
-        <v>31.48</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -1431,21 +1401,21 @@
         <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E33">
-        <v>510.19</v>
+        <v>102.1</v>
       </c>
       <c r="F33">
-        <v>1109.8900000000001</v>
+        <v>51.69</v>
       </c>
       <c r="G33">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -1454,21 +1424,21 @@
         <v>45</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E34">
-        <v>611.92999999999995</v>
+        <v>319.75</v>
       </c>
       <c r="F34">
-        <v>878.91</v>
+        <v>438.81</v>
       </c>
       <c r="G34">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
@@ -1477,21 +1447,21 @@
         <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E35">
-        <v>534.14</v>
+        <v>215.16</v>
       </c>
       <c r="F35">
-        <v>636.53</v>
+        <v>286.16</v>
       </c>
       <c r="G35">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7">
       <c r="A36" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -1500,21 +1470,21 @@
         <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E36">
-        <v>316.64</v>
+        <v>466.07</v>
       </c>
       <c r="F36">
-        <v>58.79</v>
+        <v>332.97</v>
       </c>
       <c r="G36">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7">
       <c r="A37" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
@@ -1523,21 +1493,21 @@
         <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E37">
-        <v>447.63</v>
+        <v>466.58</v>
       </c>
       <c r="F37">
-        <v>479.3</v>
+        <v>205.77</v>
       </c>
       <c r="G37">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
@@ -1546,21 +1516,21 @@
         <v>49</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E38">
-        <v>485.79</v>
+        <v>122.07</v>
       </c>
       <c r="F38">
-        <v>509.7</v>
+        <v>141.28</v>
       </c>
       <c r="G38">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7">
       <c r="A39" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
@@ -1569,21 +1539,21 @@
         <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E39">
-        <v>150.44999999999999</v>
+        <v>470.3</v>
       </c>
       <c r="F39">
-        <v>132.84</v>
+        <v>45.3</v>
       </c>
       <c r="G39">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7">
       <c r="A40" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -1592,21 +1562,21 @@
         <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E40">
-        <v>504.39</v>
+        <v>819.7</v>
       </c>
       <c r="F40">
-        <v>364.63</v>
+        <v>162.15</v>
       </c>
       <c r="G40">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7">
       <c r="A41" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
@@ -1615,21 +1585,21 @@
         <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>117.84</v>
       </c>
       <c r="F41">
-        <v>175.1</v>
+        <v>338.03</v>
       </c>
       <c r="G41">
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7">
       <c r="A42" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
@@ -1638,21 +1608,21 @@
         <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E42">
-        <v>83.91</v>
+        <v>208.07</v>
       </c>
       <c r="F42">
-        <v>673.9</v>
+        <v>242.52</v>
       </c>
       <c r="G42">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7">
       <c r="A43" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
@@ -1661,21 +1631,21 @@
         <v>54</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E43">
-        <v>165.68</v>
+        <v>-178.83</v>
       </c>
       <c r="F43">
-        <v>398.38</v>
+        <v>29.09</v>
       </c>
       <c r="G43">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7">
       <c r="A44" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -1684,21 +1654,21 @@
         <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E44">
-        <v>236.45</v>
+        <v>12.89</v>
       </c>
       <c r="F44">
-        <v>52.67</v>
+        <v>383.95</v>
       </c>
       <c r="G44">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
@@ -1707,21 +1677,21 @@
         <v>56</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E45">
-        <v>453.95</v>
+        <v>-40.5</v>
       </c>
       <c r="F45">
-        <v>597.70000000000005</v>
+        <v>360.57</v>
       </c>
       <c r="G45">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7">
       <c r="A46" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
@@ -1730,10 +1700,10 @@
         <v>57</v>
       </c>
       <c r="D46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E46">
-        <v>1575.82</v>
+        <v>2118.11</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -1742,9 +1712,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
@@ -1753,10 +1723,10 @@
         <v>58</v>
       </c>
       <c r="D47" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>293.46</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -1765,9 +1735,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7">
       <c r="A48" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
@@ -1776,21 +1746,21 @@
         <v>59</v>
       </c>
       <c r="D48" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E48">
-        <v>529.14</v>
+        <v>302.47</v>
       </c>
       <c r="F48">
-        <v>406.86</v>
+        <v>164.66</v>
       </c>
       <c r="G48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
@@ -1799,21 +1769,21 @@
         <v>60</v>
       </c>
       <c r="D49" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E49">
-        <v>232.73</v>
+        <v>-197.78</v>
       </c>
       <c r="F49">
-        <v>161.15</v>
+        <v>0</v>
       </c>
       <c r="G49">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -1822,21 +1792,21 @@
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E50">
-        <v>-296.67</v>
+        <v>90.23</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>91.20999999999999</v>
       </c>
       <c r="G50">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -1845,21 +1815,21 @@
         <v>62</v>
       </c>
       <c r="D51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>119.05</v>
       </c>
       <c r="F51">
-        <v>114.84</v>
+        <v>308.45</v>
       </c>
       <c r="G51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
@@ -1868,21 +1838,21 @@
         <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E52">
-        <v>122.07</v>
+        <v>451.35</v>
       </c>
       <c r="F52">
-        <v>330.14</v>
+        <v>391.97</v>
       </c>
       <c r="G52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -1891,21 +1861,21 @@
         <v>64</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E53">
-        <v>179.85</v>
+        <v>64.45</v>
       </c>
       <c r="F53">
-        <v>242.63</v>
+        <v>51.21</v>
       </c>
       <c r="G53">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
@@ -1914,21 +1884,21 @@
         <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E54">
-        <v>481.28</v>
+        <v>83.40000000000001</v>
       </c>
       <c r="F54">
-        <v>436.17</v>
+        <v>34.49</v>
       </c>
       <c r="G54">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -1937,21 +1907,21 @@
         <v>66</v>
       </c>
       <c r="D55" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E55">
-        <v>211.18</v>
+        <v>293.46</v>
       </c>
       <c r="F55">
-        <v>275.61</v>
+        <v>272.26</v>
       </c>
       <c r="G55">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -1960,21 +1930,21 @@
         <v>67</v>
       </c>
       <c r="D56" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E56">
-        <v>7.44</v>
+        <v>106.07</v>
       </c>
       <c r="F56">
-        <v>72.449999999999989</v>
+        <v>155.8</v>
       </c>
       <c r="G56">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B57" t="s">
         <v>11</v>
@@ -1983,21 +1953,21 @@
         <v>68</v>
       </c>
       <c r="D57" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E57">
-        <v>15.74</v>
+        <v>246.74</v>
       </c>
       <c r="F57">
-        <v>244.67</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -2006,21 +1976,21 @@
         <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E58">
-        <v>81.06</v>
+        <v>86.51000000000001</v>
       </c>
       <c r="F58">
-        <v>252.75</v>
+        <v>173.95</v>
       </c>
       <c r="G58">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
@@ -2029,21 +1999,21 @@
         <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E59">
-        <v>349</v>
+        <v>38.16</v>
       </c>
       <c r="F59">
-        <v>1102.82</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="G59">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -2052,21 +2022,21 @@
         <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E60">
-        <v>383.33</v>
+        <v>204.7</v>
       </c>
       <c r="F60">
-        <v>936</v>
+        <v>166.96</v>
       </c>
       <c r="G60">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
@@ -2075,21 +2045,21 @@
         <v>72</v>
       </c>
       <c r="D61" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E61">
-        <v>117.84</v>
+        <v>98.89</v>
       </c>
       <c r="F61">
-        <v>300.93</v>
+        <v>618.09</v>
       </c>
       <c r="G61">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -2098,21 +2068,21 @@
         <v>73</v>
       </c>
       <c r="D62" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E62">
-        <v>166.8</v>
+        <v>179.43</v>
       </c>
       <c r="F62">
-        <v>289.2</v>
+        <v>77.73999999999999</v>
       </c>
       <c r="G62">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -2121,67 +2091,67 @@
         <v>74</v>
       </c>
       <c r="D63" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E63">
-        <v>44.63</v>
+        <v>-98.89</v>
       </c>
       <c r="F63">
-        <v>421.5</v>
+        <v>0</v>
       </c>
       <c r="G63">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C64" t="s">
         <v>75</v>
       </c>
       <c r="D64" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E64">
-        <v>428.17</v>
+        <v>164.36</v>
       </c>
       <c r="F64">
-        <v>565.81999999999994</v>
+        <v>457.27</v>
       </c>
       <c r="G64">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C65" t="s">
         <v>76</v>
       </c>
       <c r="D65" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E65">
-        <v>95.68</v>
+        <v>-12.89</v>
       </c>
       <c r="F65">
-        <v>84.2</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B66" t="s">
         <v>12</v>
@@ -2190,21 +2160,21 @@
         <v>77</v>
       </c>
       <c r="D66" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E66">
-        <v>189.12</v>
+        <v>-241.39</v>
       </c>
       <c r="F66">
-        <v>517.43999999999994</v>
+        <v>224.19</v>
       </c>
       <c r="G66">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B67" t="s">
         <v>12</v>
@@ -2213,21 +2183,21 @@
         <v>78</v>
       </c>
       <c r="D67" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E67">
-        <v>435.25</v>
+        <v>210.31</v>
       </c>
       <c r="F67">
-        <v>1160.0999999999999</v>
+        <v>239.5</v>
       </c>
       <c r="G67">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B68" t="s">
         <v>12</v>
@@ -2236,21 +2206,21 @@
         <v>79</v>
       </c>
       <c r="D68" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>-107.55</v>
       </c>
       <c r="F68">
-        <v>241.82</v>
+        <v>209.75</v>
       </c>
       <c r="G68">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
@@ -2259,21 +2229,21 @@
         <v>80</v>
       </c>
       <c r="D69" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E69">
-        <v>-33.93</v>
+        <v>341.81</v>
       </c>
       <c r="F69">
-        <v>367.16</v>
+        <v>222.59</v>
       </c>
       <c r="G69">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B70" t="s">
         <v>12</v>
@@ -2282,21 +2252,21 @@
         <v>81</v>
       </c>
       <c r="D70" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E70">
-        <v>323.47000000000003</v>
+        <v>90.23</v>
       </c>
       <c r="F70">
-        <v>826.1400000000001</v>
+        <v>253.45</v>
       </c>
       <c r="G70">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
@@ -2305,21 +2275,21 @@
         <v>82</v>
       </c>
       <c r="D71" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E71">
-        <v>438.46</v>
+        <v>-88.59999999999999</v>
       </c>
       <c r="F71">
-        <v>427.94</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
@@ -2328,21 +2298,21 @@
         <v>83</v>
       </c>
       <c r="D72" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E72">
-        <v>364.58</v>
+        <v>3.21</v>
       </c>
       <c r="F72">
-        <v>233.81</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -2351,21 +2321,21 @@
         <v>84</v>
       </c>
       <c r="D73" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E73">
-        <v>382.41</v>
+        <v>360.25</v>
       </c>
       <c r="F73">
-        <v>319.83999999999997</v>
+        <v>339.11</v>
       </c>
       <c r="G73">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B74" t="s">
         <v>12</v>
@@ -2374,21 +2344,21 @@
         <v>85</v>
       </c>
       <c r="D74" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E74">
-        <v>286.73</v>
+        <v>12.89</v>
       </c>
       <c r="F74">
-        <v>728.79000000000008</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
@@ -2397,21 +2367,21 @@
         <v>86</v>
       </c>
       <c r="D75" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E75">
-        <v>50.79</v>
+        <v>-76.73</v>
       </c>
       <c r="F75">
-        <v>94.690000000000012</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
@@ -2420,21 +2390,21 @@
         <v>87</v>
       </c>
       <c r="D76" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E76">
-        <v>34.69</v>
+        <v>0</v>
       </c>
       <c r="F76">
-        <v>637.14</v>
+        <v>0</v>
       </c>
       <c r="G76">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="2">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
@@ -2443,85 +2413,16 @@
         <v>88</v>
       </c>
       <c r="D77" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E77">
-        <v>363.46</v>
+        <v>265.95</v>
       </c>
       <c r="F77">
-        <v>490.48</v>
+        <v>50.82</v>
       </c>
       <c r="G77">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="2">
-        <v>45831</v>
-      </c>
-      <c r="B78" t="s">
-        <v>12</v>
-      </c>
-      <c r="C78" t="s">
-        <v>89</v>
-      </c>
-      <c r="D78" t="s">
-        <v>93</v>
-      </c>
-      <c r="E78">
-        <v>156.51</v>
-      </c>
-      <c r="F78">
-        <v>724.85</v>
-      </c>
-      <c r="G78">
         <v>44</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" s="2">
-        <v>45831</v>
-      </c>
-      <c r="B79" t="s">
-        <v>12</v>
-      </c>
-      <c r="C79" t="s">
-        <v>90</v>
-      </c>
-      <c r="D79" t="s">
-        <v>92</v>
-      </c>
-      <c r="E79">
-        <v>-12.89</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="2">
-        <v>45831</v>
-      </c>
-      <c r="B80" t="s">
-        <v>12</v>
-      </c>
-      <c r="C80" t="s">
-        <v>91</v>
-      </c>
-      <c r="D80" t="s">
-        <v>92</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-      <c r="G80">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>